<commit_message>
Team Meeting 11/15/2020 Attendence Taken.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8C4A43-F07C-6C45-A84B-65AC30B85801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59143D1C-DA75-264E-A2B4-5C88BAC4F7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -792,7 +792,9 @@
       <c r="F17" s="6">
         <v>44144</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6">
+        <v>44150</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -819,7 +821,9 @@
       <c r="F18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -836,6 +840,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -846,6 +851,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -856,6 +862,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -866,6 +873,7 @@
       <c r="D22" s="11"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -876,6 +884,7 @@
       <c r="D23" s="11"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
+      <c r="G23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attendence Taken 11/17/2020 TA Meeting.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59143D1C-DA75-264E-A2B4-5C88BAC4F7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6863CC73-9A0A-3843-BBF1-F66EB6F8569D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +795,9 @@
       <c r="G17" s="6">
         <v>44150</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="6">
+        <v>44152</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -824,7 +826,9 @@
       <c r="G18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -841,6 +845,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -852,6 +857,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -863,6 +869,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -874,6 +881,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -885,6 +893,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="11"/>
+      <c r="H23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Attendence 11/22/2020, All Members Present.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6863CC73-9A0A-3843-BBF1-F66EB6F8569D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E88177-44DE-C04C-98DA-5AD8D62E5F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +798,9 @@
       <c r="H17" s="6">
         <v>44152</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="6">
+        <v>44157</v>
+      </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -829,7 +831,9 @@
       <c r="H18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -846,6 +850,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -858,6 +863,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -870,6 +876,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -882,6 +889,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -894,6 +902,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="11"/>
       <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attendence Taken TA Meeting 12/1/2020.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E88177-44DE-C04C-98DA-5AD8D62E5F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10316DA6-1AB8-1C4E-80AB-C255A154C3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5F142-D918-1842-A446-808F344EDBE6}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +776,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>44136</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -839,7 +839,7 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -891,7 +891,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -904,6 +904,73 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B25" s="6">
+        <v>44166</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Optional Attenence Taken For 11/23/2020.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10316DA6-1AB8-1C4E-80AB-C255A154C3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7BA1F2-ED55-5646-B65F-3166BD24E907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>TA</t>
+  </si>
+  <si>
+    <t>Blue = Sponsor was really late for meeting (no attendence required)</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +134,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -179,11 +188,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -196,10 +218,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -215,6 +240,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,15 +545,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5F142-D918-1842-A446-808F344EDBE6}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="38.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="70.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -669,7 +699,7 @@
       <c r="I9" s="6">
         <v>44129</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -701,7 +731,7 @@
       <c r="I10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -716,12 +746,12 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="11"/>
-      <c r="O11" s="9" t="s">
+      <c r="I11" s="9"/>
+      <c r="O11" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -733,11 +763,11 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="O12" s="10" t="s">
+      <c r="O12" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -749,6 +779,9 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
+      <c r="O13" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -801,7 +834,9 @@
       <c r="I17" s="6">
         <v>44157</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="6">
+        <v>44158</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
@@ -834,7 +869,9 @@
       <c r="I18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="7"/>
+      <c r="J18" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -845,18 +882,19 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -864,6 +902,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -877,6 +916,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -884,12 +924,13 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
       <c r="I22" s="5"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -897,12 +938,13 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
@@ -945,7 +987,7 @@
       <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="9"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">

</xml_diff>

<commit_message>
Attendence Taken, All Present.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7BA1F2-ED55-5646-B65F-3166BD24E907}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AB9F63-8FA1-5042-B803-82A5A1A2C376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -240,10 +240,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5F142-D918-1842-A446-808F344EDBE6}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,7 +946,9 @@
       <c r="B25" s="6">
         <v>44166</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C25" s="6">
+        <v>44171</v>
+      </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -970,7 +968,9 @@
       <c r="B26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -988,30 +988,35 @@
         <v>0</v>
       </c>
       <c r="B27" s="9"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attendence Taken Team Meeting 12/1/2020.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AB9F63-8FA1-5042-B803-82A5A1A2C376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2630EF3C-7D1D-5E46-A58B-1F381F82C08D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Spring 2021" sheetId="1" r:id="rId1"/>
+    <sheet name="Fall 2020" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -94,6 +95,12 @@
   </si>
   <si>
     <t>Blue = Sponsor was really late for meeting (no attendence required)</t>
+  </si>
+  <si>
+    <t>Spring 2021</t>
+  </si>
+  <si>
+    <t>Fall 2021</t>
   </si>
 </sst>
 </file>
@@ -109,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +144,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -225,6 +238,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5F142-D918-1842-A446-808F344EDBE6}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,83 +569,207 @@
     <col min="15" max="15" width="70.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6">
-        <v>44086</v>
-      </c>
-      <c r="C1" s="6">
-        <v>44090</v>
-      </c>
-      <c r="D1" s="6">
-        <v>44093</v>
-      </c>
-      <c r="E1" s="6">
-        <v>44096</v>
-      </c>
-      <c r="F1" s="6">
-        <v>44101</v>
-      </c>
-      <c r="G1" s="6">
-        <v>44102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>44227</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="O3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="O4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="O5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="O6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>3</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="O7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="O8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="O9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O13" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O14" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE82880-75B9-264E-8B98-088EEEFA4BC5}">
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>44086</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44090</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44093</v>
+      </c>
+      <c r="E3" s="6">
+        <v>44096</v>
+      </c>
+      <c r="F3" s="6">
+        <v>44101</v>
+      </c>
+      <c r="G3" s="6">
+        <v>44102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -637,13 +777,13 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="O5" s="3" t="s">
-        <v>6</v>
+      <c r="O5" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -652,12 +792,12 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="O6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -665,107 +805,103 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="O8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="O9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>44108</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C11" s="6">
         <v>44110</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D11" s="6">
         <v>44115</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E11" s="6">
         <v>44116</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F11" s="6">
         <v>44122</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G11" s="6">
         <v>44123</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H11" s="6">
         <v>44124</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I11" s="6">
         <v>44129</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O11" s="11" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="9"/>
-      <c r="O11" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="O12" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -774,14 +910,14 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="O13" s="14" t="s">
-        <v>19</v>
+      <c r="I13" s="9"/>
+      <c r="O13" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -791,10 +927,13 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O14" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -804,109 +943,110 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
+      <c r="O15" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="6">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19" s="6">
         <v>44136</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C19" s="6">
         <v>44137</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D19" s="6">
         <v>44138</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E19" s="6">
         <v>44143</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F19" s="6">
         <v>44144</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G19" s="6">
         <v>44150</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H19" s="6">
         <v>44152</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I19" s="6">
         <v>44157</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J19" s="6">
         <v>44158</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="10"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -916,109 +1056,140 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="10"/>
     </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="10"/>
+    </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="6">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="6">
         <v>44166</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C27" s="6">
         <v>44171</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Folder Restructure + Added Al Santillan Time Sheets.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2630EF3C-7D1D-5E46-A58B-1F381F82C08D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48034F6C-C487-554E-B27B-612579FAEA46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5F142-D918-1842-A446-808F344EDBE6}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,7 +589,6 @@
       <c r="B3" s="6">
         <v>44227</v>
       </c>
-      <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -608,6 +607,16 @@
       <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
       <c r="O4" s="2" t="s">
         <v>11</v>
       </c>
@@ -664,24 +673,59 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="6">
+        <v>44229</v>
+      </c>
       <c r="O12" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="O13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5"/>
       <c r="O14" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="O15" s="14" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Attendance For 2/7 - 2/13 Is Now Up To Date.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvaro/Documents/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarosantillan/Documents/GitHub/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48034F6C-C487-554E-B27B-612579FAEA46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A5CBB3-DEF1-794D-BD87-41ED1191EDE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring 2021" sheetId="1" r:id="rId1"/>
     <sheet name="Fall 2020" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -558,7 +558,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,6 +676,22 @@
       <c r="B12" s="6">
         <v>44229</v>
       </c>
+      <c r="C12" s="6">
+        <v>44235</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44246</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
       <c r="O12" s="12" t="s">
         <v>13</v>
       </c>
@@ -687,6 +703,22 @@
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
       <c r="O13" s="8" t="s">
         <v>14</v>
       </c>
@@ -696,6 +728,8 @@
         <v>0</v>
       </c>
       <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9"/>
       <c r="O14" s="13" t="s">
         <v>15</v>
       </c>
@@ -705,6 +739,8 @@
         <v>2</v>
       </c>
       <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="O15" s="14" t="s">
         <v>19</v>
       </c>
@@ -714,18 +750,24 @@
         <v>3</v>
       </c>
       <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Attendance Updated 2-22-2021 to 2-28-2021.
</commit_message>
<xml_diff>
--- a/Admin/Attendance/Attendence.xlsx
+++ b/Admin/Attendance/Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvarosantillan/Documents/GitHub/csci-4308-software-engineering-project-1/Admin/Attendance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34E42B3-0E70-C343-9679-46DCBB5CEE55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E256D7-36DF-0347-98EA-20F1C246A287}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" xr2:uid="{59327322-02DE-7944-89E0-21FA40C6DE20}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="22">
   <si>
     <t>Yao Siyu</t>
   </si>
@@ -558,7 +558,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H14" sqref="H14:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,8 +688,12 @@
       <c r="F12" s="6">
         <v>44243</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="6">
+        <v>44253</v>
+      </c>
+      <c r="H12" s="6">
+        <v>44253</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -719,8 +723,12 @@
       <c r="F13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -740,6 +748,8 @@
       <c r="D14" s="9"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
       <c r="O14" s="13" t="s">
         <v>15</v>
       </c>
@@ -753,6 +763,8 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="O15" s="14" t="s">
         <v>19</v>
       </c>
@@ -766,8 +778,10 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -776,8 +790,10 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -786,6 +802,8 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>